<commit_message>
minor changes to Database views
minor changes to database views before sending it to be checked.
</commit_message>
<xml_diff>
--- a/Data Analysis/Database Views.xlsx
+++ b/Data Analysis/Database Views.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0247c8816df86841/Desktop/School/Git/software-engineering-group24-25-19/Data Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2242" documentId="8_{63F981A3-F191-4218-98D5-5A08BD2DC6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18DAD6D6-A289-4350-87C4-B375CF8EECF8}"/>
+  <xr:revisionPtr revIDLastSave="2250" documentId="8_{63F981A3-F191-4218-98D5-5A08BD2DC6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBBB5FF4-9268-4BEA-A523-4E0C79A16394}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="4" xr2:uid="{7B431D7F-DEE8-43F7-8A22-B7C44A2F9D5F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="9" xr2:uid="{7B431D7F-DEE8-43F7-8A22-B7C44A2F9D5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Site Information" sheetId="10" r:id="rId1"/>
@@ -26,9 +26,6 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Raw!$N$1:$P$47</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Raw!$N$2:$N$47</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Raw!$O$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Raw!$O$2:$O$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -132,7 +129,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2482,6 +2479,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2495,6 +2497,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2508,6 +2515,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2521,6 +2533,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -2534,6 +2551,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -2547,6 +2569,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -2562,6 +2589,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -2577,6 +2609,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -2592,6 +2629,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -2607,6 +2649,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -2622,6 +2669,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -2637,6 +2689,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -2653,6 +2710,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -2669,6 +2731,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -2685,6 +2752,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -2701,6 +2773,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -2717,6 +2794,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -2733,6 +2815,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -2748,6 +2835,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -2763,6 +2855,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="20"/>
@@ -2778,6 +2875,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="21"/>
@@ -2793,6 +2895,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="22"/>
@@ -2808,6 +2915,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="23"/>
@@ -2823,6 +2935,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="24"/>
@@ -2839,6 +2956,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="25"/>
@@ -2855,6 +2977,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="26"/>
@@ -2871,6 +2998,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="27"/>
@@ -2887,6 +3019,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="28"/>
@@ -2903,6 +3040,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000039-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="29"/>
@@ -2919,6 +3061,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003B-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="30"/>
@@ -2934,6 +3081,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003D-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="31"/>
@@ -2949,6 +3101,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003F-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="32"/>
@@ -2964,6 +3121,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000041-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="33"/>
@@ -2979,6 +3141,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000043-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="34"/>
@@ -2994,6 +3161,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000045-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="35"/>
@@ -3009,6 +3181,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000047-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="36"/>
@@ -3025,6 +3202,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000049-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="37"/>
@@ -3041,6 +3223,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004B-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="38"/>
@@ -3057,6 +3244,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004D-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="39"/>
@@ -3073,6 +3265,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004F-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="40"/>
@@ -3089,6 +3286,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000051-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="41"/>
@@ -3105,6 +3307,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000053-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="42"/>
@@ -3120,6 +3327,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000055-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="43"/>
@@ -3135,6 +3347,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000057-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="44"/>
@@ -3150,6 +3367,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000059-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="45"/>
@@ -3165,6 +3387,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005B-91DE-46FE-B07D-59E24C960E1B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -3358,7 +3585,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="bestFit"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -6696,7 +6922,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6774,7 +7000,7 @@
   <dimension ref="A1:I967"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15441,12 +15667,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7A51CB-8F18-4BDE-85E6-B30889FA82D2}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="F1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19774,7 +20000,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wLPi7LnzYUMuIDhQ6cku5tbjEUZFjm8gNSZVqR30suSpMDKnI3BWKnjDtUmVA4D3C3uPYZGkroX3l7WLPqqHMA==" saltValue="cJHj4OC4WrRy7s9AwCI+Ng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="G2:G47 J2:J47 M2:M47 P2:P47 S2:S47 V2:W47">
     <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
@@ -19881,12 +20106,12 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546DB37C-57DB-4F4F-96D8-97BCCEA0E92B}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:AJ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25089,7 +25314,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="cSvEXuOVg2G99ZpPteB+h6/0UZPQpFSfY1qX2b+w0qovgzXiOIwK3QqMP5UQHxt/uFV5iHbQ4Jio999KoB28xg==" saltValue="BBIysj0n8DjGDe5yRMEEcA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="K2:K47 P2:P47 U2:U47 Z2:Z47 AE2:AE47 AJ2:AJ47">
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
@@ -25485,12 +25709,12 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC78811-0885-4871-883F-3831DECFD253}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27739,7 +27963,6 @@
     </row>
     <row r="48" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="U/o3vSeVujDkwnENWwjvPyi3dtHQAwFP1GLIJOL/caXPNSUcFaZfxIc+X2USeqMc9laWCHCggvLu9SjHiVqtng==" saltValue="lo5Y6h+TzGxJJlZ+whWC4A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="E2:E47 G2:G47 I2:I47 K2:K47 M2:M47 O2:O47">
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
@@ -33591,7 +33814,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="XCSlm/McWOi6wtCf2kLWUC79Z7Kpgw1BgrSVyQjJpkmVPsvn4GO9JC3/BmL8KtMvVv6kE0Jq8RwW+M29/Mnq+w==" saltValue="bFO20IR0Bk9xMHP/UzO3sA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -33603,7 +33825,7 @@
   </sheetPr>
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+    <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -36309,7 +36531,6 @@
       <c r="P50" s="16"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zVD1a+24JZ73Q0RxQ1cADN/6kpfOFPFn0xbQaDtjo+29zD8mxE2oGROPbj87K3y021Ynx4OC6MrHZ5kS4lAPFg==" saltValue="6a/AAObHctFX+dWL/aUATQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="N1:P47" xr:uid="{F6DE5B8C-0943-4190-90B5-8FC83F9A8F4A}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>